<commit_message>
finish dev of IAP
</commit_message>
<xml_diff>
--- a/gameData/shared/StoreItems.xlsx
+++ b/gameData/shared/StoreItems.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6520" yWindow="1680" windowWidth="25600" windowHeight="16060" tabRatio="883"/>
+    <workbookView xWindow="5760" yWindow="4060" windowWidth="25600" windowHeight="16060" tabRatio="883"/>
   </bookViews>
   <sheets>
     <sheet name="items" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
   <si>
     <t>STR_name</t>
     <phoneticPr fontId="8" type="noConversion"/>
@@ -88,6 +88,18 @@
   </si>
   <si>
     <t>STR_productId</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>INT_gem</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>STR_rewards</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>resource:woodClass_3:1,resource:stoneClass_3:1,resource:ironClass_3:1,resource:foodClass_3:1,resource:coinClass_2:1,resource:casinoTokenClass_1:1,speedup:speedup_3:2,speedup:speedup_4:1</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
@@ -231,7 +243,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="528">
+  <cellStyleXfs count="530">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0">
@@ -764,8 +776,10 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -782,17 +796,20 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="528">
+  <cellStyles count="530">
     <cellStyle name="Default 1" xfId="1"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal_" xfId="3"/>
@@ -1059,6 +1076,7 @@
     <cellStyle name="超链接" xfId="522" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="524" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="526" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="528" builtinId="8" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="15" builtinId="9" hidden="1"/>
@@ -1318,6 +1336,7 @@
     <cellStyle name="访问过的超链接" xfId="523" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="525" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="527" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="529" builtinId="9" hidden="1"/>
     <cellStyle name="解释性文本" xfId="8"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
     <cellStyle name="표준_chapter_01" xfId="9"/>
@@ -1770,13 +1789,13 @@
   <dimension ref="A1:K41"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="3" width="20.6640625" style="1"/>
-    <col min="4" max="4" width="20.6640625" style="7"/>
+    <col min="4" max="4" width="20.6640625" style="6"/>
     <col min="5" max="5" width="20.6640625" style="1"/>
     <col min="6" max="6" width="20.6640625" style="5"/>
     <col min="7" max="7" width="20.6640625" style="1"/>
@@ -1796,13 +1815,18 @@
       <c r="C1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="4"/>
+      <c r="F1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>17</v>
+      </c>
       <c r="H1" s="4"/>
       <c r="K1" s="4"/>
     </row>
@@ -1810,19 +1834,24 @@
       <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D2" s="6">
         <v>4.99</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="6"/>
+      <c r="F2" s="8">
+        <v>100</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="3" spans="1:11" ht="20" customHeight="1">
       <c r="A3" s="1">
@@ -1834,30 +1863,41 @@
       <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="6">
         <v>9.99</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>10</v>
+      </c>
+      <c r="F3" s="9">
+        <v>500</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="20" customHeight="1">
       <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="6">
         <v>19.989999999999998</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="6"/>
+      <c r="F4" s="8">
+        <v>1000</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="5" spans="1:11" ht="20" customHeight="1">
       <c r="A5" s="2">
@@ -1869,129 +1909,141 @@
       <c r="C5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="6">
         <v>49.99</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="6" t="s">
         <v>12</v>
+      </c>
+      <c r="F5" s="9">
+        <v>5000</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="20" customHeight="1">
       <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="6">
         <v>99.99</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="F6" s="9">
+        <v>10000</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="8" spans="1:11" ht="20" customHeight="1">
       <c r="A8" s="2"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
       <c r="E8" s="2"/>
     </row>
     <row r="10" spans="1:11" ht="20" customHeight="1">
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
     </row>
     <row r="11" spans="1:11" ht="20" customHeight="1">
       <c r="A11" s="2"/>
       <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:11" ht="20" customHeight="1">
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
     </row>
     <row r="14" spans="1:11" ht="20" customHeight="1">
       <c r="A14" s="2"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
       <c r="E14" s="2"/>
     </row>
     <row r="16" spans="1:11" ht="20" customHeight="1">
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
     </row>
     <row r="17" spans="1:5" ht="20" customHeight="1">
       <c r="A17" s="2"/>
       <c r="E17" s="2"/>
     </row>
     <row r="18" spans="1:5" ht="20" customHeight="1">
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
     </row>
     <row r="20" spans="1:5" ht="20" customHeight="1">
       <c r="A20" s="2"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
       <c r="E20" s="2"/>
     </row>
     <row r="22" spans="1:5" ht="20" customHeight="1">
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
     </row>
     <row r="23" spans="1:5" ht="20" customHeight="1">
       <c r="A23" s="2"/>
       <c r="E23" s="2"/>
     </row>
     <row r="24" spans="1:5" ht="20" customHeight="1">
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
     </row>
     <row r="26" spans="1:5" ht="20" customHeight="1">
       <c r="A26" s="2"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
       <c r="E26" s="2"/>
     </row>
     <row r="28" spans="1:5" ht="20" customHeight="1">
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
     </row>
     <row r="29" spans="1:5" ht="20" customHeight="1">
       <c r="A29" s="2"/>
       <c r="E29" s="2"/>
     </row>
     <row r="30" spans="1:5" ht="20" customHeight="1">
-      <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
     </row>
     <row r="32" spans="1:5" ht="20" customHeight="1">
       <c r="A32" s="2"/>
-      <c r="B32" s="7"/>
-      <c r="C32" s="7"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
       <c r="E32" s="2"/>
     </row>
     <row r="34" spans="1:5" ht="20" customHeight="1">
-      <c r="B34" s="7"/>
-      <c r="C34" s="7"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
     </row>
     <row r="35" spans="1:5" ht="20" customHeight="1">
       <c r="A35" s="2"/>
       <c r="E35" s="2"/>
     </row>
     <row r="36" spans="1:5" ht="20" customHeight="1">
-      <c r="B36" s="7"/>
-      <c r="C36" s="7"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
     </row>
     <row r="38" spans="1:5" ht="20" customHeight="1">
       <c r="A38" s="2"/>
-      <c r="B38" s="7"/>
-      <c r="C38" s="7"/>
+      <c r="B38" s="6"/>
+      <c r="C38" s="6"/>
       <c r="E38" s="2"/>
     </row>
     <row r="40" spans="1:5" ht="20" customHeight="1">
-      <c r="B40" s="7"/>
-      <c r="C40" s="7"/>
+      <c r="B40" s="6"/>
+      <c r="C40" s="6"/>
     </row>
     <row r="41" spans="1:5" ht="20" customHeight="1">
       <c r="A41" s="2"/>

</xml_diff>

<commit_message>
bugfix for storeitems config file
</commit_message>
<xml_diff>
--- a/gameData/shared/StoreItems.xlsx
+++ b/gameData/shared/StoreItems.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="980" yWindow="0" windowWidth="36820" windowHeight="16060" tabRatio="181"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21140" tabRatio="181"/>
   </bookViews>
   <sheets>
     <sheet name="items" sheetId="2" r:id="rId1"/>
@@ -143,7 +143,8 @@
     <t>special:dragonChest_3:5,special:dragonChest_2:5,special:dragonChest_1:20,resource:woodClass_6:5,resource:stoneClass_6:5,resource:ironClass_6:5,resource:foodClass_6:5,resource:coinClass_6:5,speedup:speedup_2:5,speedup:speedup_3:5,speedup:speedup_4:5,speedup:speedup_5:5,speedup:speedup_6:5,buff:woodBonus_1:5,buff:stoneBonus_1:5,buff:ironBonus_1:5,buff:foodBonus_1:5,buff:coinBonus_1:5</t>
   </si>
   <si>
-    <t>special:dragonChest_3:10,special:dragonChest_2:20,special:dragonChest_1:30,resource:woodClass_7:5,resource:stoneClass_7:5,resource:ironClass_7:5,resource:foodClass_7:5,resource:coinClass_7:5,speedup:speedup_3:5,speedup:speedup_4:5,speedup:speedup_5:5,speedup:speedup_6:5,speedup:speedup_7:5,buff:woodBonus_1:5,buff:stoneBonus_1:5,buff:ironBonus_1:5,buff:foodBonus_1:5,buff:coinBonus_1:5,buff:unitHpBonus_1:5,buff:infantryAtkBonus_1:5,buff:archerAtkBonus_1:5,buff:cavalryAtkBonus_1:,buff:siegeAtkBonus_1:5</t>
+    <t>special:dragonChest_3:10,special:dragonChest_2:20,special:dragonChest_1:30,resource:woodClass_7:5,resource:stoneClass_7:5,resource:ironClass_7:5,resource:foodClass_7:5,resource:coinClass_7:5,speedup:speedup_3:5,speedup:speedup_4:5,speedup:speedup_5:5,speedup:speedup_6:5,speedup:speedup_7:5,buff:woodBonus_1:5,buff:stoneBonus_1:5,buff:ironBonus_1:5,buff:foodBonus_1:5,buff:coinBonus_1:5,buff:unitHpBonus_1:5,buff:infantryAtkBonus_1:5,buff:archerAtkBonus_1:5,buff:cavalryAtkBonus_1:5,buff:siegeAtkBonus_1:5</t>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -286,7 +287,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="568">
+  <cellStyleXfs count="586">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0">
@@ -301,6 +302,24 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -893,7 +912,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="568">
+  <cellStyles count="586">
     <cellStyle name="Default 1" xfId="1"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal_" xfId="3"/>
@@ -1180,6 +1199,15 @@
     <cellStyle name="超链接" xfId="562" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="564" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="566" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="568" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="570" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="572" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="574" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="576" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="578" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="580" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="582" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="584" builtinId="8" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="15" builtinId="9" hidden="1"/>
@@ -1459,6 +1487,15 @@
     <cellStyle name="访问过的超链接" xfId="563" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="565" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="567" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="569" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="571" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="573" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="575" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="577" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="579" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="581" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="583" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="585" builtinId="9" hidden="1"/>
     <cellStyle name="解释性文本" xfId="8"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
     <cellStyle name="표준_chapter_01" xfId="9"/>
@@ -1911,7 +1948,7 @@
   <dimension ref="A1:K41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G6"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
dev of promotion items
</commit_message>
<xml_diff>
--- a/gameData/shared/StoreItems.xlsx
+++ b/gameData/shared/StoreItems.xlsx
@@ -1,18 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26929"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="0" windowWidth="31920" windowHeight="20460" tabRatio="181"/>
+    <workbookView xWindow="-31940" yWindow="3600" windowWidth="38400" windowHeight="21140" tabRatio="181" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="items" sheetId="2" r:id="rId1"/>
+    <sheet name="promotionItems" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="Excel_BuiltIn__FilterDatabase_2" localSheetId="1">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase_2">#REF!</definedName>
+    <definedName name="Excel_BuiltIn__FilterDatabase_6" localSheetId="1">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase_6">#REF!</definedName>
+    <definedName name="Excel_BuiltIn__FilterDatabase_7" localSheetId="1">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase_7">#REF!</definedName>
+    <definedName name="Excel_BuiltIn__FilterDatabase_8" localSheetId="1">#REF!</definedName>
     <definedName name="Excel_BuiltIn__FilterDatabase_8">#REF!</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
@@ -25,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="58">
   <si>
     <t>STR_name</t>
     <phoneticPr fontId="8" type="noConversion"/>
@@ -148,6 +153,102 @@
   </si>
   <si>
     <t>items:dragonChest_3:10,items:dragonChest_2:20,items:dragonChest_1:30,items:woodClass_7:5,items:stoneClass_7:5,items:ironClass_7:5,items:foodClass_7:5,items:coinClass_7:5,items:speedup_3:5,items:speedup_4:5,items:speedup_5:5,items:speedup_6:5,items:speedup_7:5,items:woodBonus_1:5,items:stoneBonus_1:5,items:ironBonus_1:5,items:foodBonus_1:5,items:coinBonus_1:5,items:unitHpBonus_1:5,items:infantryAtkBonus_1:5,items:archerAtkBonus_1:5,items:cavalryAtkBonus_1:5,items:siegeAtkBonus_1:5</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>远古学识特惠</t>
+  </si>
+  <si>
+    <t>promotion_product_1_1</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>promotion_product_1_2</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>promotion_product_2_1</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>promotion_product_2_2</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>promotion_product_3_1</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>promotion_product_3_2</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>promotion_product_4_1</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>promotion_product_4_2</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>com.dragonfall.promotion.15000dragoncoins</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>com.dragonfall.promotion.20000dragoncoins</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>com.dragonfall.promotion.30000dragoncoins</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>com.dragonfall.promotion.40000dragoncoins</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>com.dragonfall.promotion.80000dragoncoins</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>com.dragonfall.promotion.70000dragoncoins</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>com.dragonfall.promotion.150000dragoncoins</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>com.dragonfall.promotion.200000dragoncoins</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>富饶之地特惠</t>
+  </si>
+  <si>
+    <t>龙族宝藏特惠</t>
+  </si>
+  <si>
+    <t>好运连连特惠</t>
+  </si>
+  <si>
+    <t>贵族传承特惠</t>
+  </si>
+  <si>
+    <t>英雄之血特惠</t>
+  </si>
+  <si>
+    <t>不死军团特惠</t>
+  </si>
+  <si>
+    <t>金龙币特惠</t>
+  </si>
+  <si>
+    <t>FLOAT_promotionPercent</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>items:chest_4:3</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
@@ -291,7 +392,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="586">
+  <cellStyleXfs count="606">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0">
@@ -882,8 +983,28 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -915,8 +1036,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="586">
+  <cellStyles count="606">
     <cellStyle name="Default 1" xfId="1"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal_" xfId="3"/>
@@ -1212,6 +1360,16 @@
     <cellStyle name="超链接" xfId="580" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="582" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="584" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="586" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="588" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="590" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="592" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="594" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="596" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="598" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="600" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="602" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="604" builtinId="8" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="15" builtinId="9" hidden="1"/>
@@ -1500,6 +1658,16 @@
     <cellStyle name="访问过的超链接" xfId="581" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="583" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="585" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="587" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="589" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="591" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="593" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="595" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="597" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="599" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="601" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="603" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="605" builtinId="9" hidden="1"/>
     <cellStyle name="解释性文本" xfId="8"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
     <cellStyle name="표준_chapter_01" xfId="9"/>
@@ -1951,8 +2119,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView showRuler="0" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
@@ -2017,6 +2185,9 @@
       <c r="G2" s="10" t="s">
         <v>27</v>
       </c>
+      <c r="H2" s="5" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="3" spans="1:11" ht="65" customHeight="1">
       <c r="A3" s="1">
@@ -2041,7 +2212,7 @@
         <v>29</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="63" customHeight="1">
@@ -2067,7 +2238,7 @@
         <v>28</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="57" customHeight="1">
@@ -2093,7 +2264,7 @@
         <v>30</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="74" customHeight="1">
@@ -2119,7 +2290,7 @@
         <v>31</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>26</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="20" customHeight="1">
@@ -2225,6 +2396,399 @@
     <row r="41" spans="1:5" ht="20" customHeight="1">
       <c r="A41" s="2"/>
       <c r="E41" s="2"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="3" width="20.6640625" style="18"/>
+    <col min="4" max="4" width="20.6640625" style="15"/>
+    <col min="5" max="5" width="20.6640625" style="18"/>
+    <col min="6" max="7" width="16.1640625" style="17" customWidth="1"/>
+    <col min="8" max="8" width="217.33203125" style="18" customWidth="1"/>
+    <col min="9" max="9" width="20.6640625" style="17"/>
+    <col min="10" max="11" width="20.6640625" style="18"/>
+    <col min="12" max="12" width="20.6640625" style="17"/>
+    <col min="13" max="16384" width="20.6640625" style="18"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="11" customFormat="1" ht="20" customHeight="1">
+      <c r="A1" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" s="13"/>
+    </row>
+    <row r="2" spans="1:12" ht="58" customHeight="1">
+      <c r="A2" s="14">
+        <v>1</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" s="15">
+        <v>9.99</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="16">
+        <v>15000</v>
+      </c>
+      <c r="G2" s="16">
+        <v>4.5549999999999997</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" s="17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="65" customHeight="1">
+      <c r="A3" s="18">
+        <v>2</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" s="15">
+        <v>9.99</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3" s="19">
+        <v>20000</v>
+      </c>
+      <c r="G3" s="19">
+        <v>4.6449999999999996</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="I3" s="17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="63" customHeight="1">
+      <c r="A4" s="18">
+        <v>3</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" s="15">
+        <v>19.989999999999998</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="16">
+        <v>30000</v>
+      </c>
+      <c r="G4" s="16">
+        <v>4.79</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" s="17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="57" customHeight="1">
+      <c r="A5" s="14">
+        <v>4</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="15">
+        <v>19.989999999999998</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" s="19">
+        <v>40000</v>
+      </c>
+      <c r="G5" s="19">
+        <v>4.8324999999999996</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I5" s="17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="74" customHeight="1">
+      <c r="A6" s="18">
+        <v>5</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" s="15">
+        <v>49.99</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="F6" s="19">
+        <v>80000</v>
+      </c>
+      <c r="G6" s="19">
+        <v>5.0519999999999996</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="I6" s="17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="49" customHeight="1">
+      <c r="A7" s="14">
+        <v>6</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" s="15">
+        <v>49.99</v>
+      </c>
+      <c r="E7" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="F7" s="19">
+        <v>70000</v>
+      </c>
+      <c r="G7" s="19">
+        <v>5.093</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="I7" s="17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="50" customHeight="1">
+      <c r="A8" s="18">
+        <v>7</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="D8" s="15">
+        <v>99.99</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="F8" s="19">
+        <v>150000</v>
+      </c>
+      <c r="G8" s="19">
+        <v>5.5339999999999998</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="I8" s="17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="47" customHeight="1">
+      <c r="A9" s="14">
+        <v>8</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" s="15">
+        <v>99.99</v>
+      </c>
+      <c r="E9" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="F9" s="19">
+        <v>200000</v>
+      </c>
+      <c r="G9" s="19">
+        <v>5.6050000000000004</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="I9" s="17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="20" customHeight="1">
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+    </row>
+    <row r="11" spans="1:12" ht="20" customHeight="1">
+      <c r="A11" s="14"/>
+      <c r="E11" s="14"/>
+    </row>
+    <row r="12" spans="1:12" ht="20" customHeight="1">
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+    </row>
+    <row r="14" spans="1:12" ht="20" customHeight="1">
+      <c r="A14" s="14"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+      <c r="E14" s="14"/>
+    </row>
+    <row r="16" spans="1:12" ht="20" customHeight="1">
+      <c r="B16" s="15"/>
+      <c r="C16" s="15"/>
+    </row>
+    <row r="17" spans="1:5" ht="20" customHeight="1">
+      <c r="A17" s="14"/>
+      <c r="E17" s="14"/>
+    </row>
+    <row r="18" spans="1:5" ht="20" customHeight="1">
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
+    </row>
+    <row r="20" spans="1:5" ht="20" customHeight="1">
+      <c r="A20" s="14"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
+      <c r="E20" s="14"/>
+    </row>
+    <row r="22" spans="1:5" ht="20" customHeight="1">
+      <c r="B22" s="15"/>
+      <c r="C22" s="15"/>
+    </row>
+    <row r="23" spans="1:5" ht="20" customHeight="1">
+      <c r="A23" s="14"/>
+      <c r="E23" s="14"/>
+    </row>
+    <row r="24" spans="1:5" ht="20" customHeight="1">
+      <c r="B24" s="15"/>
+      <c r="C24" s="15"/>
+    </row>
+    <row r="26" spans="1:5" ht="20" customHeight="1">
+      <c r="A26" s="14"/>
+      <c r="B26" s="15"/>
+      <c r="C26" s="15"/>
+      <c r="E26" s="14"/>
+    </row>
+    <row r="28" spans="1:5" ht="20" customHeight="1">
+      <c r="B28" s="15"/>
+      <c r="C28" s="15"/>
+    </row>
+    <row r="29" spans="1:5" ht="20" customHeight="1">
+      <c r="A29" s="14"/>
+      <c r="E29" s="14"/>
+    </row>
+    <row r="30" spans="1:5" ht="20" customHeight="1">
+      <c r="B30" s="15"/>
+      <c r="C30" s="15"/>
+    </row>
+    <row r="32" spans="1:5" ht="20" customHeight="1">
+      <c r="A32" s="14"/>
+      <c r="B32" s="15"/>
+      <c r="C32" s="15"/>
+      <c r="E32" s="14"/>
+    </row>
+    <row r="34" spans="1:5" ht="20" customHeight="1">
+      <c r="B34" s="15"/>
+      <c r="C34" s="15"/>
+    </row>
+    <row r="35" spans="1:5" ht="20" customHeight="1">
+      <c r="A35" s="14"/>
+      <c r="E35" s="14"/>
+    </row>
+    <row r="36" spans="1:5" ht="20" customHeight="1">
+      <c r="B36" s="15"/>
+      <c r="C36" s="15"/>
+    </row>
+    <row r="38" spans="1:5" ht="20" customHeight="1">
+      <c r="A38" s="14"/>
+      <c r="B38" s="15"/>
+      <c r="C38" s="15"/>
+      <c r="E38" s="14"/>
+    </row>
+    <row r="40" spans="1:5" ht="20" customHeight="1">
+      <c r="B40" s="15"/>
+      <c r="C40" s="15"/>
+    </row>
+    <row r="41" spans="1:5" ht="20" customHeight="1">
+      <c r="A41" s="14"/>
+      <c r="E41" s="14"/>
     </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>

</xml_diff>